<commit_message>
Added old sql scripts. Working on flat_data.sql
</commit_message>
<xml_diff>
--- a/ETL Concepts.xlsx
+++ b/ETL Concepts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\ETL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\etl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1900" windowWidth="19200" windowHeight="7520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2280" windowWidth="19200" windowHeight="7520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>HIV WESTERN BLOT, QUALITATIVE</t>
   </si>
   <si>
-    <t>western_blot</t>
-  </si>
-  <si>
     <t>a899afec-1350-11df-a1f1-0026b9348838</t>
   </si>
   <si>
@@ -1424,6 +1421,9 @@
   </si>
   <si>
     <t>on pcp prophy</t>
+  </si>
+  <si>
+    <t>hiv_western_blot</t>
   </si>
 </sst>
 </file>
@@ -3362,15 +3362,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B4" s="7">
         <v>19</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B5" s="7">
         <v>14</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B6" s="7">
         <v>17</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B7" s="7">
         <v>26</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B8" s="7">
         <v>14</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B9" s="7">
         <v>6</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B10" s="7">
         <v>3</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B11" s="7">
         <v>17</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B13" s="7">
         <v>27</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B14" s="7">
         <v>144</v>
@@ -3465,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3491,19 +3491,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>434</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J1" s="3"/>
     </row>
@@ -3512,20 +3512,20 @@
         <v>1192</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H2" t="str">
         <f>IF(E2=TRUE,
@@ -3553,22 +3553,22 @@
         <v>1087</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(E3=TRUE,
@@ -3596,22 +3596,22 @@
         <v>1088</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3627,20 +3627,20 @@
         <v>1156</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3656,20 +3656,20 @@
         <v>1164</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3685,22 +3685,22 @@
         <v>1250</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3716,20 +3716,20 @@
         <v>1251</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3745,20 +3745,20 @@
         <v>1252</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3774,20 +3774,20 @@
         <v>1255</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3803,20 +3803,20 @@
         <v>1490</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3832,20 +3832,20 @@
         <v>1505</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -3861,20 +3861,20 @@
         <v>1717</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -3890,20 +3890,20 @@
         <v>1999</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3919,22 +3919,22 @@
         <v>2031</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -3950,20 +3950,20 @@
         <v>2033</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -3979,22 +3979,22 @@
         <v>2154</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -4010,20 +4010,20 @@
         <v>2155</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>340</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -4039,22 +4039,22 @@
         <v>2157</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>342</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>343</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -4070,22 +4070,22 @@
         <v>1187</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -4101,20 +4101,20 @@
         <v>1387</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -4136,16 +4136,16 @@
         <v>37</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -4161,22 +4161,22 @@
         <v>1086</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -4192,22 +4192,22 @@
         <v>1147</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -4223,22 +4223,22 @@
         <v>1176</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -4254,20 +4254,20 @@
         <v>1181</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -4283,20 +4283,20 @@
         <v>1499</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -4312,20 +4312,20 @@
         <v>1719</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -4338,553 +4338,781 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
-        <v>12</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
+        <v>654</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=12,value_coded,null)) as chest_xray,</v>
+        <f>IF(E29=TRUE,
+  "group_concat(if(concept_id="&amp;A29&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D29&amp;",",
+   "min(if(concept_id="&amp;A29&amp;",value_"&amp;F29&amp;",null)) as "&amp;D29&amp;",")</f>
+        <v>min(if(concept_id=654,value_numeric,null)) as alt,</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="1"/>
-        <v>chest_xray int,</v>
+        <f>IF(E29=TRUE,
+D29&amp;" varchar(1000),",
+IF(F29="coded",D29&amp;" int,",
+IF(F29="numeric",D29&amp;" double,",
+IF(F29="datetime",D29&amp;" datetime,",
+IF(F29="boolean",D29&amp;" boolean,",
+IF(F29="text",D29&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>alt double,</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
-        <v>45</v>
+        <v>653</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=45,value_coded,null)) as urine_pregnancy_test,</v>
+        <f>IF(E30=TRUE,
+  "group_concat(if(concept_id="&amp;A30&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D30&amp;",",
+   "min(if(concept_id="&amp;A30&amp;",value_"&amp;F30&amp;",null)) as "&amp;D30&amp;",")</f>
+        <v>min(if(concept_id=653,value_numeric,null)) as ast,</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="1"/>
-        <v>urine_pregnancy_test int,</v>
+        <f>IF(E30=TRUE,
+D30&amp;" varchar(1000),",
+IF(F30="coded",D30&amp;" int,",
+IF(F30="numeric",D30&amp;" double,",
+IF(F30="datetime",D30&amp;" datetime,",
+IF(F30="boolean",D30&amp;" boolean,",
+IF(F30="text",D30&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>ast double,</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
-        <v>299</v>
+        <v>5497</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>369</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>370</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>15</v>
+        <v>372</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=299,value_coded,null)) as vdrl,</v>
+        <f>IF(E31=TRUE,
+  "group_concat(if(concept_id="&amp;A31&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D31&amp;",",
+   "min(if(concept_id="&amp;A31&amp;",value_"&amp;F31&amp;",null)) as "&amp;D31&amp;",")</f>
+        <v>min(if(concept_id=5497,value_numeric,null)) as cd4_count,</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="1"/>
-        <v>vdrl int,</v>
+        <f>IF(E31=TRUE,
+D31&amp;" varchar(1000),",
+IF(F31="coded",D31&amp;" int,",
+IF(F31="numeric",D31&amp;" double,",
+IF(F31="datetime",D31&amp;" datetime,",
+IF(F31="boolean",D31&amp;" boolean,",
+IF(F31="text",D31&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>cd4_count double,</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <v>307</v>
+        <v>730</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=307,value_coded,null)) as sputum_afb,</v>
+        <f>IF(E32=TRUE,
+  "group_concat(if(concept_id="&amp;A32&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D32&amp;",",
+   "min(if(concept_id="&amp;A32&amp;",value_"&amp;F32&amp;",null)) as "&amp;D32&amp;",")</f>
+        <v>min(if(concept_id=730,value_numeric,null)) as cd4_percent,</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="1"/>
-        <v>sputum_afb int,</v>
+        <f>IF(E32=TRUE,
+D32&amp;" varchar(1000),",
+IF(F32="coded",D32&amp;" int,",
+IF(F32="numeric",D32&amp;" double,",
+IF(F32="datetime",D32&amp;" datetime,",
+IF(F32="boolean",D32&amp;" boolean,",
+IF(F32="text",D32&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>cd4_percent double,</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
-        <v>1030</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1030,value_coded,null)) as hiv_dna_pcr,</v>
+        <f>IF(E33=TRUE,
+  "group_concat(if(concept_id="&amp;A33&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D33&amp;",",
+   "min(if(concept_id="&amp;A33&amp;",value_"&amp;F33&amp;",null)) as "&amp;D33&amp;",")</f>
+        <v>min(if(concept_id=12,value_coded,null)) as chest_xray,</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="1"/>
-        <v>hiv_dna_pcr int,</v>
+        <f>IF(E33=TRUE,
+D33&amp;" varchar(1000),",
+IF(F33="coded",D33&amp;" int,",
+IF(F33="numeric",D33&amp;" double,",
+IF(F33="datetime",D33&amp;" datetime,",
+IF(F33="boolean",D33&amp;" boolean,",
+IF(F33="text",D33&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>chest_xray int,</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
-        <v>1031</v>
+        <v>790</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1031,value_coded,null)) as syphylis_tpha_titer,</v>
+        <f>IF(E34=TRUE,
+  "group_concat(if(concept_id="&amp;A34&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D34&amp;",",
+   "min(if(concept_id="&amp;A34&amp;",value_"&amp;F34&amp;",null)) as "&amp;D34&amp;",")</f>
+        <v>min(if(concept_id=790,value_numeric,null)) as creatinine,</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="1"/>
-        <v>syphylis_tpha_titer int,</v>
+        <f>IF(E34=TRUE,
+D34&amp;" varchar(1000),",
+IF(F34="coded",D34&amp;" int,",
+IF(F34="numeric",D34&amp;" double,",
+IF(F34="datetime",D34&amp;" datetime,",
+IF(F34="boolean",D34&amp;" boolean,",
+IF(F34="text",D34&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>creatinine double,</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
-        <v>1032</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1032,value_coded,null)) as syphylis_tpha_qual,</v>
+        <f>IF(E35=TRUE,
+  "group_concat(if(concept_id="&amp;A35&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D35&amp;",",
+   "min(if(concept_id="&amp;A35&amp;",value_"&amp;F35&amp;",null)) as "&amp;D35&amp;",")</f>
+        <v>min(if(concept_id=21,value_numeric,null)) as hemoglobin,</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="1"/>
-        <v>syphylis_tpha_qual int,</v>
+        <f>IF(E35=TRUE,
+D35&amp;" varchar(1000),",
+IF(F35="coded",D35&amp;" int,",
+IF(F35="numeric",D35&amp;" double,",
+IF(F35="datetime",D35&amp;" datetime,",
+IF(F35="boolean",D35&amp;" boolean,",
+IF(F35="text",D35&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hemoglobin double,</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
-        <v>1039</v>
+        <v>1030</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1039,value_coded,null)) as tv_pcr,</v>
+        <f>IF(E36=TRUE,
+  "group_concat(if(concept_id="&amp;A36&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D36&amp;",",
+   "min(if(concept_id="&amp;A36&amp;",value_"&amp;F36&amp;",null)) as "&amp;D36&amp;",")</f>
+        <v>min(if(concept_id=1030,value_coded,null)) as hiv_dna_pcr,</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="1"/>
-        <v>tv_pcr int,</v>
+        <f>IF(E36=TRUE,
+D36&amp;" varchar(1000),",
+IF(F36="coded",D36&amp;" int,",
+IF(F36="numeric",D36&amp;" double,",
+IF(F36="datetime",D36&amp;" datetime,",
+IF(F36="boolean",D36&amp;" boolean,",
+IF(F36="text",D36&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hiv_dna_pcr int,</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1040,value_coded,null)) as hiv_rapid_test,</v>
+        <f>IF(E37=TRUE,
+  "group_concat(if(concept_id="&amp;A37&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D37&amp;",",
+   "min(if(concept_id="&amp;A37&amp;",value_"&amp;F37&amp;",null)) as "&amp;D37&amp;",")</f>
+        <v>min(if(concept_id=1042,value_coded,null)) as hiv_long_elisa,</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="1"/>
-        <v>hiv_rapid_test int,</v>
+        <f>IF(E37=TRUE,
+D37&amp;" varchar(1000),",
+IF(F37="coded",D37&amp;" int,",
+IF(F37="numeric",D37&amp;" double,",
+IF(F37="datetime",D37&amp;" datetime,",
+IF(F37="boolean",D37&amp;" boolean,",
+IF(F37="text",D37&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hiv_long_elisa int,</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1042,value_coded,null)) as hiv_long_elisa,</v>
+        <f>IF(E38=TRUE,
+  "group_concat(if(concept_id="&amp;A38&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D38&amp;",",
+   "min(if(concept_id="&amp;A38&amp;",value_"&amp;F38&amp;",null)) as "&amp;D38&amp;",")</f>
+        <v>min(if(concept_id=1040,value_coded,null)) as hiv_rapid_test,</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="1"/>
-        <v>hiv_long_elisa int,</v>
+        <f>IF(E38=TRUE,
+D38&amp;" varchar(1000),",
+IF(F38="coded",D38&amp;" int,",
+IF(F38="numeric",D38&amp;" double,",
+IF(F38="datetime",D38&amp;" datetime,",
+IF(F38="boolean",D38&amp;" boolean,",
+IF(F38="text",D38&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hiv_rapid_test int,</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
-        <v>1047</v>
+        <v>1305</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>194</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>58</v>
+        <v>195</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1047,value_coded,null)) as western_blot,</v>
+        <f>IF(E39=TRUE,
+  "group_concat(if(concept_id="&amp;A39&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D39&amp;",",
+   "min(if(concept_id="&amp;A39&amp;",value_"&amp;F39&amp;",null)) as "&amp;D39&amp;",")</f>
+        <v>min(if(concept_id=1305,value_coded,null)) as hiv_vl_qual,</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="1"/>
-        <v>western_blot int,</v>
+        <f>IF(E39=TRUE,
+D39&amp;" varchar(1000),",
+IF(F39="coded",D39&amp;" int,",
+IF(F39="numeric",D39&amp;" double,",
+IF(F39="datetime",D39&amp;" datetime,",
+IF(F39="boolean",D39&amp;" boolean,",
+IF(F39="text",D39&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hiv_vl_qual int,</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
-        <v>1305</v>
+        <v>1047</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>196</v>
+        <v>58</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>197</v>
+        <v>463</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=1305,value_coded,null)) as hiv_vl_qual,</v>
+        <f>IF(E40=TRUE,
+  "group_concat(if(concept_id="&amp;A40&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D40&amp;",",
+   "min(if(concept_id="&amp;A40&amp;",value_"&amp;F40&amp;",null)) as "&amp;D40&amp;",")</f>
+        <v>min(if(concept_id=1047,value_coded,null)) as hiv_western_blot,</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="1"/>
-        <v>hiv_vl_qual int,</v>
+        <f>IF(E40=TRUE,
+D40&amp;" varchar(1000),",
+IF(F40="coded",D40&amp;" int,",
+IF(F40="numeric",D40&amp;" double,",
+IF(F40="datetime",D40&amp;" datetime,",
+IF(F40="boolean",D40&amp;" boolean,",
+IF(F40="text",D40&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>hiv_western_blot int,</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
-        <v>21</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>7</v>
+        <v>307</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=21,value_numeric,null)) as hemoglobin,</v>
+        <f>IF(E41=TRUE,
+  "group_concat(if(concept_id="&amp;A41&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D41&amp;",",
+   "min(if(concept_id="&amp;A41&amp;",value_"&amp;F41&amp;",null)) as "&amp;D41&amp;",")</f>
+        <v>min(if(concept_id=307,value_coded,null)) as sputum_afb,</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="1"/>
-        <v>hemoglobin double,</v>
+        <f>IF(E41=TRUE,
+D41&amp;" varchar(1000),",
+IF(F41="coded",D41&amp;" int,",
+IF(F41="numeric",D41&amp;" double,",
+IF(F41="datetime",D41&amp;" datetime,",
+IF(F41="boolean",D41&amp;" boolean,",
+IF(F41="text",D41&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>sputum_afb int,</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
-        <v>653</v>
+        <v>1032</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=653,value_numeric,null)) as ast,</v>
+        <f>IF(E42=TRUE,
+  "group_concat(if(concept_id="&amp;A42&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D42&amp;",",
+   "min(if(concept_id="&amp;A42&amp;",value_"&amp;F42&amp;",null)) as "&amp;D42&amp;",")</f>
+        <v>min(if(concept_id=1032,value_coded,null)) as syphylis_tpha_qual,</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="1"/>
-        <v>ast double,</v>
+        <f>IF(E42=TRUE,
+D42&amp;" varchar(1000),",
+IF(F42="coded",D42&amp;" int,",
+IF(F42="numeric",D42&amp;" double,",
+IF(F42="datetime",D42&amp;" datetime,",
+IF(F42="boolean",D42&amp;" boolean,",
+IF(F42="text",D42&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>syphylis_tpha_qual int,</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
-        <v>654</v>
+        <v>1031</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=654,value_numeric,null)) as alt,</v>
+        <f>IF(E43=TRUE,
+  "group_concat(if(concept_id="&amp;A43&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D43&amp;",",
+   "min(if(concept_id="&amp;A43&amp;",value_"&amp;F43&amp;",null)) as "&amp;D43&amp;",")</f>
+        <v>min(if(concept_id=1031,value_coded,null)) as syphylis_tpha_titer,</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="1"/>
-        <v>alt double,</v>
+        <f>IF(E43=TRUE,
+D43&amp;" varchar(1000),",
+IF(F43="coded",D43&amp;" int,",
+IF(F43="numeric",D43&amp;" double,",
+IF(F43="datetime",D43&amp;" datetime,",
+IF(F43="boolean",D43&amp;" boolean,",
+IF(F43="text",D43&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>syphylis_tpha_titer int,</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>730</v>
+        <v>1039</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=730,value_numeric,null)) as cd4_percent,</v>
+        <f>IF(E44=TRUE,
+  "group_concat(if(concept_id="&amp;A44&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D44&amp;",",
+   "min(if(concept_id="&amp;A44&amp;",value_"&amp;F44&amp;",null)) as "&amp;D44&amp;",")</f>
+        <v>min(if(concept_id=1039,value_coded,null)) as tv_pcr,</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="1"/>
-        <v>cd4_percent double,</v>
+        <f>IF(E44=TRUE,
+D44&amp;" varchar(1000),",
+IF(F44="coded",D44&amp;" int,",
+IF(F44="numeric",D44&amp;" double,",
+IF(F44="datetime",D44&amp;" datetime,",
+IF(F44="boolean",D44&amp;" boolean,",
+IF(F44="text",D44&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>tv_pcr int,</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
-        <v>790</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=790,value_numeric,null)) as creatinine,</v>
+        <f>IF(E45=TRUE,
+  "group_concat(if(concept_id="&amp;A45&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D45&amp;",",
+   "min(if(concept_id="&amp;A45&amp;",value_"&amp;F45&amp;",null)) as "&amp;D45&amp;",")</f>
+        <v>min(if(concept_id=45,value_coded,null)) as urine_pregnancy_test,</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="1"/>
-        <v>creatinine double,</v>
+        <f>IF(E45=TRUE,
+D45&amp;" varchar(1000),",
+IF(F45="coded",D45&amp;" int,",
+IF(F45="numeric",D45&amp;" double,",
+IF(F45="datetime",D45&amp;" datetime,",
+IF(F45="boolean",D45&amp;" boolean,",
+IF(F45="text",D45&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>urine_pregnancy_test int,</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
-        <v>856</v>
+        <v>299</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=856,value_numeric,null)) as viral_load,</v>
+        <f>IF(E46=TRUE,
+  "group_concat(if(concept_id="&amp;A46&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D46&amp;",",
+   "min(if(concept_id="&amp;A46&amp;",value_"&amp;F46&amp;",null)) as "&amp;D46&amp;",")</f>
+        <v>min(if(concept_id=299,value_coded,null)) as vdrl,</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="1"/>
-        <v>viral_load double,</v>
+        <f>IF(E46=TRUE,
+D46&amp;" varchar(1000),",
+IF(F46="coded",D46&amp;" int,",
+IF(F46="numeric",D46&amp;" double,",
+IF(F46="datetime",D46&amp;" datetime,",
+IF(F46="boolean",D46&amp;" boolean,",
+IF(F46="text",D46&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>vdrl int,</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
-        <v>5497</v>
+        <v>856</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>370</v>
+        <v>34</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>371</v>
+        <v>35</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>373</v>
+        <v>36</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="0"/>
-        <v>min(if(concept_id=5497,value_numeric,null)) as cd4_count,</v>
+        <f>IF(E47=TRUE,
+  "group_concat(if(concept_id="&amp;A47&amp;",value_coded,null) order by value_coded separator ' // ') as "&amp;D47&amp;",",
+   "min(if(concept_id="&amp;A47&amp;",value_"&amp;F47&amp;",null)) as "&amp;D47&amp;",")</f>
+        <v>min(if(concept_id=856,value_numeric,null)) as viral_load,</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="1"/>
-        <v>cd4_count double,</v>
+        <f>IF(E47=TRUE,
+D47&amp;" varchar(1000),",
+IF(F47="coded",D47&amp;" int,",
+IF(F47="numeric",D47&amp;" double,",
+IF(F47="datetime",D47&amp;" datetime,",
+IF(F47="boolean",D47&amp;" boolean,",
+IF(F47="text",D47&amp;" varchar(1000),","")
+)
+)
+)
+))</f>
+        <v>viral_load double,</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -4892,20 +5120,20 @@
         <v>1109</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -4921,20 +5149,20 @@
         <v>1112</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -4950,22 +5178,22 @@
         <v>1193</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="E50" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -4981,20 +5209,20 @@
         <v>1261</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -5010,20 +5238,20 @@
         <v>1263</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -5039,20 +5267,20 @@
         <v>1277</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -5068,20 +5296,20 @@
         <v>1278</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -5097,22 +5325,22 @@
         <v>1637</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="E55" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -5128,22 +5356,22 @@
         <v>1668</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="E56" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -5159,22 +5387,22 @@
         <v>1879</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="E57" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -5190,22 +5418,22 @@
         <v>1895</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="E58" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -5221,20 +5449,20 @@
         <v>2250</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -5250,22 +5478,22 @@
         <v>8346</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>429</v>
       </c>
       <c r="E60" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -5281,20 +5509,20 @@
         <v>1246</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -5310,20 +5538,20 @@
         <v>1361</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -5339,22 +5567,22 @@
         <v>1271</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="E63" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -5370,20 +5598,20 @@
         <v>1285</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -5399,20 +5627,20 @@
         <v>1357</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -5428,20 +5656,20 @@
         <v>1591</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
@@ -5467,20 +5695,20 @@
         <v>1596</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H131" si="3">IF(E67=TRUE,
@@ -5498,22 +5726,22 @@
         <v>1705</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="E68" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="3"/>
@@ -5529,22 +5757,22 @@
         <v>1733</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="E69" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="3"/>
@@ -5560,22 +5788,22 @@
         <v>1834</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="E70" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="3"/>
@@ -5591,22 +5819,22 @@
         <v>1835</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="E71" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="3"/>
@@ -5622,20 +5850,20 @@
         <v>1839</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="3"/>
@@ -5651,20 +5879,20 @@
         <v>7015</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="3" t="s">
         <v>422</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>423</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="3"/>
@@ -5680,20 +5908,20 @@
         <v>1502</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="3"/>
@@ -5709,20 +5937,20 @@
         <v>1568</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="3"/>
@@ -5738,20 +5966,20 @@
         <v>5096</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>358</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="3"/>
@@ -5767,20 +5995,20 @@
         <v>7016</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>426</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="3"/>
@@ -5796,20 +6024,20 @@
         <v>1942</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="3"/>
@@ -5825,20 +6053,20 @@
         <v>1943</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="3"/>
@@ -5854,20 +6082,20 @@
         <v>2020</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="3"/>
@@ -5883,20 +6111,20 @@
         <v>1248</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="3"/>
@@ -5922,10 +6150,10 @@
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="3"/>
@@ -5941,20 +6169,20 @@
         <v>1061</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="3"/>
@@ -5970,22 +6198,22 @@
         <v>1071</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E84" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="3"/>
@@ -6001,22 +6229,22 @@
         <v>1078</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E85" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="3"/>
@@ -6032,22 +6260,22 @@
         <v>1080</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E86" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="3"/>
@@ -6063,22 +6291,22 @@
         <v>1492</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="E87" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="3"/>
@@ -6094,22 +6322,22 @@
         <v>1493</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="E88" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="3"/>
@@ -6125,22 +6353,22 @@
         <v>1790</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="E89" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="3"/>
@@ -6156,20 +6384,20 @@
         <v>1946</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="3"/>
@@ -6185,20 +6413,20 @@
         <v>5271</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>361</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="3"/>
@@ -6214,20 +6442,20 @@
         <v>5356</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="3"/>
@@ -6243,20 +6471,20 @@
         <v>5958</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>385</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="3"/>
@@ -6272,20 +6500,20 @@
         <v>5959</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="3"/>
@@ -6301,20 +6529,20 @@
         <v>5971</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>394</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="3"/>
@@ -6330,20 +6558,20 @@
         <v>5984</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>397</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="3"/>
@@ -6359,22 +6587,22 @@
         <v>6042</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>403</v>
       </c>
       <c r="E97" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="3"/>
@@ -6390,20 +6618,20 @@
         <v>6048</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>406</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="3"/>
@@ -6419,22 +6647,22 @@
         <v>6802</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="3" t="s">
         <v>419</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>420</v>
       </c>
       <c r="E99" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="3"/>
@@ -6450,20 +6678,20 @@
         <v>9082</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="3"/>
@@ -6479,20 +6707,20 @@
         <v>6796</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="D101" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="3"/>
@@ -6508,20 +6736,20 @@
         <v>5089</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>352</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="3"/>
@@ -6537,20 +6765,20 @@
         <v>5090</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="3" t="s">
         <v>354</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>355</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="3"/>
@@ -6566,20 +6794,20 @@
         <v>1573</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H104" t="str">
         <f>IF(E104=TRUE,
@@ -6607,20 +6835,20 @@
         <v>1734</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H105" t="str">
         <f>IF(E105=TRUE,
@@ -6648,20 +6876,20 @@
         <v>1570</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H106" t="str">
         <f>IF(E106=TRUE,
@@ -6689,20 +6917,20 @@
         <v>1856</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="3"/>
@@ -6718,20 +6946,20 @@
         <v>5272</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>364</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="3"/>
@@ -6747,22 +6975,22 @@
         <v>1363</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="D109" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="E109" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="3"/>
@@ -6778,20 +7006,20 @@
         <v>1846</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="3"/>
@@ -6807,20 +7035,20 @@
         <v>1992</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="3"/>
@@ -6836,20 +7064,20 @@
         <v>2055</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="3"/>
@@ -6865,20 +7093,20 @@
         <v>2198</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="3" t="s">
         <v>345</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>346</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="3"/>
@@ -6894,20 +7122,20 @@
         <v>5630</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="3"/>
@@ -6923,20 +7151,20 @@
         <v>1836</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D115" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="3"/>
@@ -6952,20 +7180,20 @@
         <v>5596</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>376</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="3"/>
@@ -6981,20 +7209,20 @@
         <v>5599</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>379</v>
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="3"/>
@@ -7010,20 +7238,20 @@
         <v>1279</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="3"/>
@@ -7039,20 +7267,20 @@
         <v>1855</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="3"/>
@@ -7068,20 +7296,20 @@
         <v>5992</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>400</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="3"/>
@@ -7097,20 +7325,20 @@
         <v>1146</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>458</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>459</v>
       </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="3"/>
@@ -7126,22 +7354,22 @@
         <v>1208</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="E122" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="3"/>
@@ -7157,20 +7385,20 @@
         <v>1209</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="3"/>
@@ -7186,20 +7414,20 @@
         <v>1224</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="D124" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="3"/>
@@ -7215,22 +7443,22 @@
         <v>1225</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E125" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="3"/>
@@ -7246,20 +7474,20 @@
         <v>2019</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="3"/>
@@ -7275,20 +7503,20 @@
         <v>5303</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D127" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="E127" s="3"/>
       <c r="F127" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="3"/>
@@ -7304,20 +7532,20 @@
         <v>2021</v>
       </c>
       <c r="B128" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="3"/>
@@ -7333,20 +7561,20 @@
         <v>2022</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="E129" s="3"/>
       <c r="F129" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="3"/>
@@ -7362,20 +7590,20 @@
         <v>1110</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="D130" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="3"/>
@@ -7391,22 +7619,22 @@
         <v>1111</v>
       </c>
       <c r="B131" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E131" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H131" t="str">
         <f t="shared" si="3"/>
@@ -7432,20 +7660,20 @@
         <v>1264</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" ref="H132:H144" si="5">IF(E132=TRUE,
@@ -7463,20 +7691,20 @@
         <v>1265</v>
       </c>
       <c r="B133" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="E133" s="3"/>
       <c r="F133" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" si="5"/>
@@ -7492,20 +7720,20 @@
         <v>1266</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="E134" s="3"/>
       <c r="F134" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="5"/>
@@ -7521,20 +7749,20 @@
         <v>1268</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E135" s="3"/>
       <c r="F135" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="5"/>
@@ -7550,20 +7778,20 @@
         <v>1269</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="D136" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E136" s="3"/>
       <c r="F136" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="5"/>
@@ -7579,22 +7807,22 @@
         <v>1270</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="D137" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="E137" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="5"/>
@@ -7610,20 +7838,20 @@
         <v>1506</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="E138" s="3"/>
       <c r="F138" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="5"/>
@@ -7639,20 +7867,20 @@
         <v>2028</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>326</v>
       </c>
       <c r="E139" s="3"/>
       <c r="F139" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" si="5"/>
@@ -7668,20 +7896,20 @@
         <v>5965</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="D140" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="E140" s="3"/>
       <c r="F140" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="5"/>
@@ -7697,20 +7925,20 @@
         <v>6077</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="E141" s="3"/>
       <c r="F141" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" si="5"/>
@@ -7726,22 +7954,22 @@
         <v>6174</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="E142" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" si="5"/>
@@ -7757,20 +7985,20 @@
         <v>6206</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="E143" s="3"/>
       <c r="F143" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="5"/>
@@ -7786,20 +8014,20 @@
         <v>1113</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E144" s="3"/>
       <c r="F144" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="5"/>
@@ -7815,13 +8043,13 @@
         <v>1085</v>
       </c>
       <c r="B145" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
@@ -7839,8 +8067,8 @@
       <sortCondition ref="G1:G145"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:A270">
-    <sortCondition ref="A2:A270"/>
+  <sortState ref="A29:I47">
+    <sortCondition ref="D29:D47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7859,22 +8087,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added lab indicators to moh 731 indicators
</commit_message>
<xml_diff>
--- a/ETL Concepts.xlsx
+++ b/ETL Concepts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2660" windowWidth="19200" windowHeight="7520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3040" windowWidth="19200" windowHeight="7520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>HIV VIRAL LOAD, QUANTITATIVE</t>
   </si>
   <si>
-    <t>viral_load</t>
-  </si>
-  <si>
     <t>CURRENT ANTIRETROVIRAL DRUGS USED FOR TRANSMISSION PROPHYLAXIS</t>
   </si>
   <si>
@@ -1424,6 +1421,9 @@
   </si>
   <si>
     <t>current_meds</t>
+  </si>
+  <si>
+    <t>hiv_vl_quant</t>
   </si>
 </sst>
 </file>
@@ -3362,15 +3362,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B4" s="7">
         <v>19</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B5" s="7">
         <v>14</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B6" s="7">
         <v>17</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B7" s="7">
         <v>26</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B8" s="7">
         <v>14</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B9" s="7">
         <v>6</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="7">
         <v>3</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B11" s="7">
         <v>17</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B13" s="7">
         <v>27</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B14" s="7">
         <v>144</v>
@@ -3465,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3491,19 +3491,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>432</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J1" s="3"/>
     </row>
@@ -3512,20 +3512,20 @@
         <v>1192</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H2" t="str">
         <f>IF(E2=TRUE,
@@ -3553,22 +3553,22 @@
         <v>1087</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(E3=TRUE,
@@ -3596,22 +3596,22 @@
         <v>1088</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3627,20 +3627,20 @@
         <v>1156</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3656,20 +3656,20 @@
         <v>1164</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3685,22 +3685,22 @@
         <v>1250</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3716,20 +3716,20 @@
         <v>1251</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3745,20 +3745,20 @@
         <v>1252</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3774,20 +3774,20 @@
         <v>1255</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3803,20 +3803,20 @@
         <v>1490</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3832,20 +3832,20 @@
         <v>1505</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -3861,20 +3861,20 @@
         <v>1717</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -3890,20 +3890,20 @@
         <v>1999</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3919,22 +3919,22 @@
         <v>2031</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -3950,20 +3950,20 @@
         <v>2033</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -3979,22 +3979,22 @@
         <v>2154</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -4010,20 +4010,20 @@
         <v>2155</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -4039,22 +4039,22 @@
         <v>2157</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -4070,22 +4070,22 @@
         <v>1187</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -4101,20 +4101,20 @@
         <v>1387</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -4130,22 +4130,22 @@
         <v>966</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -4161,22 +4161,22 @@
         <v>1086</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -4192,22 +4192,22 @@
         <v>1147</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -4223,22 +4223,22 @@
         <v>1176</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -4254,20 +4254,20 @@
         <v>1181</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -4283,20 +4283,20 @@
         <v>1499</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -4312,20 +4312,20 @@
         <v>1719</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -4351,10 +4351,10 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" ref="H29:H47" si="2">IF(E29=TRUE,
@@ -4392,10 +4392,10 @@
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
@@ -4411,20 +4411,20 @@
         <v>5497</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
@@ -4450,10 +4450,10 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
@@ -4479,10 +4479,10 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
@@ -4508,10 +4508,10 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="2"/>
@@ -4537,10 +4537,10 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
@@ -4556,20 +4556,20 @@
         <v>1030</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
@@ -4585,20 +4585,20 @@
         <v>1042</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
@@ -4614,20 +4614,20 @@
         <v>1040</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
@@ -4643,20 +4643,20 @@
         <v>1305</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
@@ -4672,20 +4672,20 @@
         <v>1047</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="2"/>
@@ -4711,10 +4711,10 @@
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="2"/>
@@ -4730,20 +4730,20 @@
         <v>1032</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="2"/>
@@ -4759,20 +4759,20 @@
         <v>1031</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="2"/>
@@ -4788,20 +4788,20 @@
         <v>1039</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="2"/>
@@ -4827,10 +4827,10 @@
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="2"/>
@@ -4856,10 +4856,10 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="2"/>
@@ -4881,22 +4881,22 @@
         <v>35</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>36</v>
+        <v>463</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="2"/>
-        <v>min(if(concept_id=856,value_numeric,null)) as viral_load,</v>
+        <v>min(if(concept_id=856,value_numeric,null)) as hiv_vl_quant,</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="3"/>
-        <v>viral_load double,</v>
+        <v>hiv_vl_quant double,</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -4904,20 +4904,20 @@
         <v>1109</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -4933,20 +4933,20 @@
         <v>1112</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -4962,22 +4962,22 @@
         <v>1193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E50" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -4993,20 +4993,20 @@
         <v>1261</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -5022,20 +5022,20 @@
         <v>1263</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -5051,20 +5051,20 @@
         <v>1277</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -5080,20 +5080,20 @@
         <v>1278</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -5109,22 +5109,22 @@
         <v>1637</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="E55" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -5140,22 +5140,22 @@
         <v>1668</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="E56" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -5171,22 +5171,22 @@
         <v>1879</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="E57" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -5202,22 +5202,22 @@
         <v>1895</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="E58" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -5233,20 +5233,20 @@
         <v>2250</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -5262,22 +5262,22 @@
         <v>8346</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>427</v>
       </c>
       <c r="E60" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -5293,20 +5293,20 @@
         <v>1246</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -5322,20 +5322,20 @@
         <v>1361</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -5351,22 +5351,22 @@
         <v>1271</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="E63" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -5382,20 +5382,20 @@
         <v>1285</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -5411,20 +5411,20 @@
         <v>1357</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -5440,20 +5440,20 @@
         <v>1591</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
@@ -5479,20 +5479,20 @@
         <v>1596</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H131" si="5">IF(E67=TRUE,
@@ -5510,22 +5510,22 @@
         <v>1705</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="E68" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="5"/>
@@ -5541,22 +5541,22 @@
         <v>1733</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="E69" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="5"/>
@@ -5572,22 +5572,22 @@
         <v>1834</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="E70" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="5"/>
@@ -5603,22 +5603,22 @@
         <v>1835</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="E71" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="5"/>
@@ -5634,20 +5634,20 @@
         <v>1839</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="5"/>
@@ -5663,20 +5663,20 @@
         <v>7015</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>421</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="5"/>
@@ -5692,20 +5692,20 @@
         <v>1502</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="5"/>
@@ -5721,20 +5721,20 @@
         <v>1568</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="5"/>
@@ -5750,20 +5750,20 @@
         <v>5096</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="5"/>
@@ -5779,20 +5779,20 @@
         <v>7016</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>424</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="5"/>
@@ -5808,20 +5808,20 @@
         <v>1942</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="5"/>
@@ -5837,20 +5837,20 @@
         <v>1943</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="5"/>
@@ -5866,20 +5866,20 @@
         <v>2020</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="5"/>
@@ -5895,20 +5895,20 @@
         <v>1248</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="5"/>
@@ -5934,10 +5934,10 @@
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="5"/>
@@ -5953,20 +5953,20 @@
         <v>1061</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="5"/>
@@ -5982,22 +5982,22 @@
         <v>1071</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E84" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="5"/>
@@ -6013,22 +6013,22 @@
         <v>1078</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E85" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="5"/>
@@ -6044,22 +6044,22 @@
         <v>1080</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E86" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="5"/>
@@ -6075,22 +6075,22 @@
         <v>1492</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="E87" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="5"/>
@@ -6106,22 +6106,22 @@
         <v>1493</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E88" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="5"/>
@@ -6137,22 +6137,22 @@
         <v>1790</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="E89" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="5"/>
@@ -6168,20 +6168,20 @@
         <v>1946</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="5"/>
@@ -6197,20 +6197,20 @@
         <v>5271</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="3" t="s">
         <v>358</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>359</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="5"/>
@@ -6226,20 +6226,20 @@
         <v>5356</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="5"/>
@@ -6255,20 +6255,20 @@
         <v>5958</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>383</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="5"/>
@@ -6284,20 +6284,20 @@
         <v>5959</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="5"/>
@@ -6313,20 +6313,20 @@
         <v>5971</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="5"/>
@@ -6342,20 +6342,20 @@
         <v>5984</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>395</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="5"/>
@@ -6371,22 +6371,22 @@
         <v>6042</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="E97" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="5"/>
@@ -6402,20 +6402,20 @@
         <v>6048</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="5"/>
@@ -6431,22 +6431,22 @@
         <v>6802</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>418</v>
       </c>
       <c r="E99" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="5"/>
@@ -6462,20 +6462,20 @@
         <v>9082</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="3" t="s">
         <v>429</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>430</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="5"/>
@@ -6491,20 +6491,20 @@
         <v>6796</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>415</v>
-      </c>
       <c r="D101" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="5"/>
@@ -6520,20 +6520,20 @@
         <v>5089</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="5"/>
@@ -6549,20 +6549,20 @@
         <v>5090</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>353</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="5"/>
@@ -6578,20 +6578,20 @@
         <v>1573</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H104" t="str">
         <f>IF(E104=TRUE,
@@ -6619,20 +6619,20 @@
         <v>1734</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H105" t="str">
         <f>IF(E105=TRUE,
@@ -6660,20 +6660,20 @@
         <v>1570</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H106" t="str">
         <f>IF(E106=TRUE,
@@ -6701,20 +6701,20 @@
         <v>1856</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="5"/>
@@ -6730,20 +6730,20 @@
         <v>5272</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="5"/>
@@ -6759,22 +6759,22 @@
         <v>1363</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="D109" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="E109" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="5"/>
@@ -6790,20 +6790,20 @@
         <v>1846</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="5"/>
@@ -6819,20 +6819,20 @@
         <v>1992</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="5"/>
@@ -6848,20 +6848,20 @@
         <v>2055</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="5"/>
@@ -6877,20 +6877,20 @@
         <v>2198</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="3" t="s">
         <v>343</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="5"/>
@@ -6906,20 +6906,20 @@
         <v>5630</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="5"/>
@@ -6935,20 +6935,20 @@
         <v>1836</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D115" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="5"/>
@@ -6964,20 +6964,20 @@
         <v>5596</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>374</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="5"/>
@@ -6993,20 +6993,20 @@
         <v>5599</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>377</v>
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="5"/>
@@ -7022,20 +7022,20 @@
         <v>1279</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="5"/>
@@ -7051,20 +7051,20 @@
         <v>1855</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="5"/>
@@ -7080,20 +7080,20 @@
         <v>5992</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="5"/>
@@ -7109,20 +7109,20 @@
         <v>1146</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>457</v>
       </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="5"/>
@@ -7138,22 +7138,22 @@
         <v>1208</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E122" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="5"/>
@@ -7169,20 +7169,20 @@
         <v>1209</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="5"/>
@@ -7198,20 +7198,20 @@
         <v>1224</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="D124" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="5"/>
@@ -7227,22 +7227,22 @@
         <v>1225</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="E125" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="5"/>
@@ -7258,20 +7258,20 @@
         <v>2019</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>312</v>
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="5"/>
@@ -7287,20 +7287,20 @@
         <v>5303</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D127" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>365</v>
       </c>
       <c r="E127" s="3"/>
       <c r="F127" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="5"/>
@@ -7316,20 +7316,20 @@
         <v>2021</v>
       </c>
       <c r="B128" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="5"/>
@@ -7345,20 +7345,20 @@
         <v>2022</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="E129" s="3"/>
       <c r="F129" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="5"/>
@@ -7374,20 +7374,20 @@
         <v>1110</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="D130" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="5"/>
@@ -7403,22 +7403,22 @@
         <v>1111</v>
       </c>
       <c r="B131" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="E131" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H131" t="str">
         <f t="shared" si="5"/>
@@ -7444,20 +7444,20 @@
         <v>1264</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" ref="H132:H144" si="7">IF(E132=TRUE,
@@ -7475,20 +7475,20 @@
         <v>1265</v>
       </c>
       <c r="B133" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="E133" s="3"/>
       <c r="F133" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" si="7"/>
@@ -7504,20 +7504,20 @@
         <v>1266</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="E134" s="3"/>
       <c r="F134" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="7"/>
@@ -7533,20 +7533,20 @@
         <v>1268</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E135" s="3"/>
       <c r="F135" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="7"/>
@@ -7562,20 +7562,20 @@
         <v>1269</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="D136" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E136" s="3"/>
       <c r="F136" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="7"/>
@@ -7591,22 +7591,22 @@
         <v>1270</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="D137" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="E137" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="7"/>
@@ -7622,20 +7622,20 @@
         <v>1506</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="E138" s="3"/>
       <c r="F138" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="7"/>
@@ -7651,20 +7651,20 @@
         <v>2028</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>324</v>
       </c>
       <c r="E139" s="3"/>
       <c r="F139" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" si="7"/>
@@ -7680,20 +7680,20 @@
         <v>5965</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="D140" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>389</v>
       </c>
       <c r="E140" s="3"/>
       <c r="F140" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="7"/>
@@ -7709,20 +7709,20 @@
         <v>6077</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="3" t="s">
         <v>406</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>407</v>
       </c>
       <c r="E141" s="3"/>
       <c r="F141" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" si="7"/>
@@ -7738,22 +7738,22 @@
         <v>6174</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="E142" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" si="7"/>
@@ -7769,20 +7769,20 @@
         <v>6206</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="3" t="s">
         <v>412</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="E143" s="3"/>
       <c r="F143" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="7"/>
@@ -7798,20 +7798,20 @@
         <v>1113</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E144" s="3"/>
       <c r="F144" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="7"/>
@@ -7827,13 +7827,13 @@
         <v>1085</v>
       </c>
       <c r="B145" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
@@ -7871,22 +7871,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>